<commit_message>
prep for performance test 8 threads 2xlarge. cloudformation template on S3.
</commit_message>
<xml_diff>
--- a/aws/aws-costing.xlsx
+++ b/aws/aws-costing.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/frankang/lab/packer/aws/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E4A836A-8CBF-B145-A945-29FE3F527F55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B35EBF1-FF73-BE46-9406-68C9E50B685D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12560" yWindow="4940" windowWidth="18740" windowHeight="14660" xr2:uid="{83AB4EB4-CE1A-CD40-A505-C7CB07160AD2}"/>
+    <workbookView xWindow="1040" yWindow="2820" windowWidth="23200" windowHeight="16780" xr2:uid="{83AB4EB4-CE1A-CD40-A505-C7CB07160AD2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="68">
   <si>
     <t>Data size</t>
   </si>
@@ -64,61 +64,181 @@
     <t>Packing</t>
   </si>
   <si>
-    <t>Data Transfer - online option</t>
-  </si>
-  <si>
-    <t>AWS egress cost to Internet per GiB</t>
-  </si>
-  <si>
-    <t>AWS total egress cost to Internet.</t>
-  </si>
-  <si>
-    <t>TODO VERIFY</t>
-  </si>
-  <si>
-    <t>AWS egress cost to On-Premises over DX per GiB</t>
-  </si>
-  <si>
-    <t>AWS total egress cost to On-Premises over DX</t>
-  </si>
-  <si>
-    <t>Time required Hours</t>
-  </si>
-  <si>
-    <t>Time required Days</t>
-  </si>
-  <si>
-    <t>Time required Hours over 1Gpbs</t>
-  </si>
-  <si>
     <t xml:space="preserve">AWS EC2 r5d.2xlarge cost </t>
   </si>
   <si>
-    <t>AWS DX port cost</t>
-  </si>
-  <si>
-    <t>DX partner cost</t>
-  </si>
-  <si>
-    <t>Assume sunk cost</t>
-  </si>
-  <si>
     <t>Total AWS EC2+EBS cost</t>
   </si>
   <si>
-    <t xml:space="preserve">AWS EBS gp3 cost (TODO? GB) </t>
-  </si>
-  <si>
-    <t>Time required days over 1Gpbs</t>
-  </si>
-  <si>
-    <t>Data Transfer - offline option</t>
-  </si>
-  <si>
     <t>Data Transfer - offline option, shipping.</t>
   </si>
   <si>
     <t>Sneakernet vendor rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AWS EC2 r5d.2xlarge hourly cost </t>
+  </si>
+  <si>
+    <t>hourly instance cost</t>
+  </si>
+  <si>
+    <t>AWS EBS gp3 per-volume size GB</t>
+  </si>
+  <si>
+    <t>AWS EBS gp3 total cost</t>
+  </si>
+  <si>
+    <t>Duration Hours</t>
+  </si>
+  <si>
+    <t>Duration Days</t>
+  </si>
+  <si>
+    <t>GB-month</t>
+  </si>
+  <si>
+    <t>AWS EBS gp3 per-GB month</t>
+  </si>
+  <si>
+    <t>AWS egress cost to Internet (1PiB)</t>
+  </si>
+  <si>
+    <t>per GB</t>
+  </si>
+  <si>
+    <t>Data Transfer total cost</t>
+  </si>
+  <si>
+    <t>Sneakernet total</t>
+  </si>
+  <si>
+    <t>Duration hours over 1Gpbs</t>
+  </si>
+  <si>
+    <t>Duration days over 1Gpbs</t>
+  </si>
+  <si>
+    <t>Staging storage</t>
+  </si>
+  <si>
+    <t>Number of 32GB CAR files</t>
+  </si>
+  <si>
+    <t>https://calculator.aws/#/estimate?id=37e2efbf7f6e7392ca4fb38e6bb7fbfd36488900</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>1PiB S3 website</t>
+  </si>
+  <si>
+    <t>1 PB Amazon Elastic File System (EFS)</t>
+  </si>
+  <si>
+    <t>S3 website option, 30 days</t>
+  </si>
+  <si>
+    <t>EFS and EC2 option</t>
+  </si>
+  <si>
+    <t>Includes CAR generation and 1-copy data transfer out</t>
+  </si>
+  <si>
+    <t>Monthly</t>
+  </si>
+  <si>
+    <t>Annual</t>
+  </si>
+  <si>
+    <t>S3 Standard 1PiB</t>
+  </si>
+  <si>
+    <t>S3 Glacier Deep Archive 1PiB</t>
+  </si>
+  <si>
+    <t>Data Transfer 1PiB out to Internet</t>
+  </si>
+  <si>
+    <t>https://calculator.aws/#/estimate?id=22b7ec1b4a92bbc1f7b710b3376ae446347c58d7</t>
+  </si>
+  <si>
+    <t>https://calculator.aws/#/estimate?id=5a12ce740f233a9068ced6a14a876fc5c7f120a5</t>
+  </si>
+  <si>
+    <t>1-time Total cost for Packer 1PiB and offline egress</t>
+  </si>
+  <si>
+    <t>1-time Total cost for Packer 1PiB and online egress</t>
+  </si>
+  <si>
+    <t>Total Packer Cost</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Amazon EC2 m6g.xlarge</t>
+  </si>
+  <si>
+    <t>https://calculator.aws/#/estimate?id=fce962bba0bec7424e12e5d3768652ca49ca247f</t>
+  </si>
+  <si>
+    <t>Data transfer out over DX from US regions rate.</t>
+  </si>
+  <si>
+    <t>Data transfer out over DX from US regions.</t>
+  </si>
+  <si>
+    <t>DX 1Gbps port hour cost</t>
+  </si>
+  <si>
+    <t>AWS Packer Costing</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Region assumption: US East (Ohio)</t>
+  </si>
+  <si>
+    <t>Data Transfer out, Online option</t>
+  </si>
+  <si>
+    <t>Data Transfer out: Offline option (DX to on-prem)</t>
+  </si>
+  <si>
+    <t>Cost of doing nothing</t>
+  </si>
+  <si>
+    <t>S3 Glacier Deep Archive option</t>
+  </si>
+  <si>
+    <t>S3 Standard option</t>
+  </si>
+  <si>
+    <t>On-demand with auto termination on job completion.</t>
+  </si>
+  <si>
+    <t>DX port cost monthly (730 h)</t>
+  </si>
+  <si>
+    <t>DX port cost for duration.</t>
+  </si>
+  <si>
+    <t>DX Partner costs</t>
+  </si>
+  <si>
+    <t>Potentially treated as sunk cost.</t>
+  </si>
+  <si>
+    <t>https://calculator.aws/#/estimate?id=4c16c04377580680bbb563a194b15e332593cc8b</t>
+  </si>
+  <si>
+    <t>Depends on provider. Possibly treated as sunk cost.</t>
+  </si>
+  <si>
+    <t>Depends on provider. Plug in actual estimates.</t>
+  </si>
+  <si>
+    <t>Data Transfer Out</t>
+  </si>
+  <si>
+    <t>1 full retrieval each month. Retrievals and Data Transfer form bulk of cost.</t>
   </si>
 </sst>
 </file>
@@ -127,10 +247,10 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0"/>
-    <numFmt numFmtId="177" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0.000_);_(&quot;$&quot;* \(#,##0.000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -153,13 +273,45 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -171,20 +323,77 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="3"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="44" fontId="1" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -497,10 +706,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84EBD14C-2462-924E-BF35-38DE282BD9FC}">
-  <dimension ref="A2:C27"/>
+  <dimension ref="A1:C60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="129" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="129" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -509,212 +718,526 @@
     <col min="2" max="2" width="13.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="7"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2">
+      <c r="B4" s="33">
         <f>1024*1024</f>
         <v>1048576</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="10">
+        <f>B4/32</f>
+        <v>32768</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="7"/>
+      <c r="B6" s="10"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B5">
+      <c r="B8">
         <v>120</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C8" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B6">
+      <c r="B9">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B7">
-        <f>B5*B6</f>
+      <c r="B10">
+        <f>B8*B9</f>
         <v>1200</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C10" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="3">
+        <f>B4/B10</f>
+        <v>873.81333333333339</v>
+      </c>
+      <c r="C11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="3">
+        <f>B11/24</f>
+        <v>36.408888888888889</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="5">
+        <v>0.57599999999999996</v>
+      </c>
+      <c r="C13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="2">
+        <f>B11*B13*B9</f>
+        <v>5033.1648000000005</v>
+      </c>
+      <c r="C14" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="3">
-        <f>B2/B7</f>
-        <v>873.81333333333339</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="B15" s="6">
+        <v>500</v>
+      </c>
+      <c r="C15" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2">
+        <f>B15*B9*B16*B12/30</f>
+        <v>606.81481481481489</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" s="34">
+        <f>B14+B17</f>
+        <v>5639.9796148148152</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="7"/>
+      <c r="B19" s="9"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" s="9"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" s="9"/>
+      <c r="C21" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" s="32">
+        <v>23322.7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" s="4"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" s="4">
+        <v>115.42</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25" s="4">
+        <v>26214.400000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="B26" s="27">
+        <f>B24+B25</f>
+        <v>26329.82</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="20"/>
+      <c r="B27" s="31"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B28" s="14"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="B29" s="4"/>
+      <c r="C29" s="11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="B30" s="26">
+        <v>56320</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="B31" s="4"/>
+      <c r="C31" s="11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="B32" s="3">
+        <f>(B4*8)/(60*60)</f>
+        <v>2330.1688888888889</v>
+      </c>
+      <c r="C32" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="3">
-        <f>B8/24</f>
-        <v>36.408888888888889</v>
-      </c>
-      <c r="C9" t="s">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="B33" s="3">
+        <f>B32/24</f>
+        <v>97.090370370370366</v>
+      </c>
+      <c r="C33" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="3"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="B34" s="15">
+        <v>0.02</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="B35" s="15">
+        <f>B34*B4</f>
+        <v>20971.52</v>
+      </c>
+      <c r="C35" s="8"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="B36" s="24">
+        <v>0.3</v>
+      </c>
+      <c r="C36" s="8"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="B37" s="24">
+        <f>B36*730</f>
+        <v>219</v>
+      </c>
+      <c r="C37" s="8"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="B38" s="24">
+        <f>B37*B33/30</f>
+        <v>708.75970370370362</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="B39" s="14">
+        <v>0</v>
+      </c>
+      <c r="C39" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="3"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" s="4">
-        <f>B10+B11</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B13" s="3"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15" s="2">
-        <v>0.03</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="B40" s="23">
+        <f>B35+B38</f>
+        <v>21680.279703703705</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="B41" s="21"/>
+      <c r="C41" s="13"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" s="29" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>11</v>
-      </c>
-      <c r="B16" s="2">
-        <f>B2*B15</f>
-        <v>31457.279999999999</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>13</v>
-      </c>
-      <c r="B19" s="2">
-        <v>0.01</v>
-      </c>
-      <c r="C19" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>14</v>
-      </c>
-      <c r="B20" s="2">
-        <f>B2*B19</f>
-        <v>10485.76</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>17</v>
-      </c>
-      <c r="B21" s="3">
-        <f>(B2*8)/(60*60)</f>
-        <v>2330.1688888888889</v>
-      </c>
-      <c r="C21" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+      <c r="B42" s="21">
+        <v>1000</v>
+      </c>
+      <c r="C42" s="25" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="3">
-        <f>B21/24</f>
-        <v>97.090370370370366</v>
-      </c>
-      <c r="C22" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>19</v>
-      </c>
-      <c r="B23" s="5">
-        <v>0</v>
-      </c>
-      <c r="C23" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>20</v>
-      </c>
-      <c r="B24" s="5">
-        <v>0</v>
-      </c>
-      <c r="C24" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="1"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>27</v>
+      <c r="B43" s="30">
+        <f>B42</f>
+        <v>1000</v>
+      </c>
+      <c r="C43" s="13"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" s="13"/>
+      <c r="B44" s="14"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="B45" s="4"/>
+      <c r="C45" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="B46" s="17">
+        <f>B18+B22+B40</f>
+        <v>50642.959318518522</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="B47" s="23">
+        <f>B18+B22+B30</f>
+        <v>85282.679614814813</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" s="18"/>
+      <c r="B48" s="14"/>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B49" s="4"/>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="B50" s="4"/>
+      <c r="C50" s="11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B51" s="4">
+        <v>23317.3</v>
+      </c>
+      <c r="C51" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B52" s="4">
+        <v>56320</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B53" s="16">
+        <v>78343.41</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B54" s="16">
+        <v>940120.92</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" s="13"/>
+      <c r="B55" s="4"/>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="B56" s="4"/>
+      <c r="C56" s="11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B57" s="4">
+        <v>23322.7</v>
+      </c>
+      <c r="C57" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B58" s="4">
+        <v>56320</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B59" s="16">
+        <v>79642.7</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B60" s="16">
+        <v>955712.4</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C21" r:id="rId1" location="/estimate?id=37e2efbf7f6e7392ca4fb38e6bb7fbfd36488900" xr:uid="{D9E540A8-05AB-AF40-92F7-9FAFFAF8F41C}"/>
+    <hyperlink ref="C50" r:id="rId2" location="/estimate?id=22b7ec1b4a92bbc1f7b710b3376ae446347c58d7" xr:uid="{FC4F9CBF-A486-ED47-92E7-7421BF4DDAD7}"/>
+    <hyperlink ref="C56" r:id="rId3" location="/estimate?id=5a12ce740f233a9068ced6a14a876fc5c7f120a5" xr:uid="{8AD7C63D-2EA5-D446-A5E7-49A132EB98CC}"/>
+    <hyperlink ref="C29" r:id="rId4" location="/estimate?id=fce962bba0bec7424e12e5d3768652ca49ca247f" xr:uid="{6E0B54C5-B977-9544-A421-4036910D2B49}"/>
+    <hyperlink ref="C31" r:id="rId5" location="/estimate?id=4c16c04377580680bbb563a194b15e332593cc8b" xr:uid="{C21B7998-CD83-C14F-BAAB-FC2495D789DB}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
aws costing doc, make 200GiB test data, appliance jobs=6
</commit_message>
<xml_diff>
--- a/aws/aws-costing.xlsx
+++ b/aws/aws-costing.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/frankang/lab/packer/aws/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B35EBF1-FF73-BE46-9406-68C9E50B685D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E4B38C6-4BEA-9546-85FC-BEA5C9985F81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1040" yWindow="2820" windowWidth="23200" windowHeight="16780" xr2:uid="{83AB4EB4-CE1A-CD40-A505-C7CB07160AD2}"/>
+    <workbookView xWindow="1040" yWindow="2820" windowWidth="23200" windowHeight="16780" activeTab="1" xr2:uid="{83AB4EB4-CE1A-CD40-A505-C7CB07160AD2}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Costing appliance" sheetId="1" r:id="rId1"/>
+    <sheet name="Performance" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="83">
   <si>
     <t>Data size</t>
   </si>
@@ -239,16 +240,63 @@
   </si>
   <si>
     <t>1 full retrieval each month. Retrievals and Data Transfer form bulk of cost.</t>
+  </si>
+  <si>
+    <t>real    49m45.579s</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>GiB</t>
+  </si>
+  <si>
+    <t>1 day</t>
+  </si>
+  <si>
+    <t>1MiB</t>
+  </si>
+  <si>
+    <t>1KiB</t>
+  </si>
+  <si>
+    <t>1GiB</t>
+  </si>
+  <si>
+    <t>File size</t>
+  </si>
+  <si>
+    <t>10GiB</t>
+  </si>
+  <si>
+    <t>GiB per file</t>
+  </si>
+  <si>
+    <t>Count</t>
+  </si>
+  <si>
+    <t>Data Set per bin</t>
+  </si>
+  <si>
+    <t>Bin Count</t>
+  </si>
+  <si>
+    <t>Total Data Set</t>
+  </si>
+  <si>
+    <t>Bin size</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="5">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0.000_);_(&quot;$&quot;* \(#,##0.000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="167" formatCode="0.000E+00"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -282,7 +330,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -313,6 +361,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -328,7 +382,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -390,6 +444,10 @@
     <xf numFmtId="164" fontId="1" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="44" fontId="1" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -708,7 +766,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84EBD14C-2462-924E-BF35-38DE282BD9FC}">
   <dimension ref="A1:C60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="129" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A44" zoomScale="129" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
@@ -1240,4 +1298,180 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{232E8F86-D048-3747-9BA9-E7C963FAAE8E}">
+  <dimension ref="B2:F23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B3">
+        <v>49</v>
+      </c>
+      <c r="C3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D3">
+        <v>100</v>
+      </c>
+      <c r="E3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B4">
+        <v>60</v>
+      </c>
+      <c r="C4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D4" s="36">
+        <f>D3*60/B3</f>
+        <v>122.44897959183673</v>
+      </c>
+      <c r="E4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D5" s="36">
+        <f>D4*24</f>
+        <v>2938.7755102040815</v>
+      </c>
+      <c r="E5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>75</v>
+      </c>
+      <c r="C13" t="s">
+        <v>77</v>
+      </c>
+      <c r="D13" t="s">
+        <v>78</v>
+      </c>
+      <c r="E13" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>73</v>
+      </c>
+      <c r="C14">
+        <f>1/1024/1024</f>
+        <v>9.5367431640625E-7</v>
+      </c>
+      <c r="D14" s="38">
+        <v>1000</v>
+      </c>
+      <c r="E14" s="37">
+        <f>C14*D14</f>
+        <v>9.5367431640625E-4</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>72</v>
+      </c>
+      <c r="C15">
+        <f>1/1024</f>
+        <v>9.765625E-4</v>
+      </c>
+      <c r="D15" s="38">
+        <v>500</v>
+      </c>
+      <c r="E15" s="37">
+        <f t="shared" ref="E15:E17" si="0">C15*D15</f>
+        <v>0.48828125</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>74</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16" s="38">
+        <v>23</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>76</v>
+      </c>
+      <c r="C17">
+        <v>10</v>
+      </c>
+      <c r="D17" s="38">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>82</v>
+      </c>
+      <c r="E21" s="36">
+        <f>SUM(E14:E20)</f>
+        <v>33.489234924316406</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>80</v>
+      </c>
+      <c r="E22">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
+        <v>81</v>
+      </c>
+      <c r="E23" s="35">
+        <f>E21*E22</f>
+        <v>200.93540954589844</v>
+      </c>
+      <c r="F23" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>